<commit_message>
Partially working snake game.
</commit_message>
<xml_diff>
--- a/_CONTROL_MAPPINGS_TEST.xlsx
+++ b/_CONTROL_MAPPINGS_TEST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSE_CourseMaterials\CSES 210 - ARCHITECTURE SESSIONAL\MIPS_Assignment_03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E83B6-C263-4226-B079-9AD37292EA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D2FDFB-0224-4EE5-A768-87CB81D8FE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
   <si>
     <t>Binary</t>
   </si>
@@ -210,22 +210,31 @@
     <t>DATA + STACK</t>
   </si>
   <si>
-    <t>#ef</t>
-  </si>
-  <si>
     <t>#ff</t>
   </si>
   <si>
-    <t>#f0</t>
-  </si>
-  <si>
     <t>Memory Layout Mapping (Binary)</t>
   </si>
   <si>
     <t>I/O PERIPHERAL</t>
   </si>
   <si>
-    <t>#</t>
+    <t>#af</t>
+  </si>
+  <si>
+    <t>SNAKE BODY</t>
+  </si>
+  <si>
+    <t>FROM</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>#c0</t>
+  </si>
+  <si>
+    <t>#a0</t>
   </si>
 </sst>
 </file>
@@ -643,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AE26"/>
+  <dimension ref="B2:AH26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +675,7 @@
     <col min="31" max="31" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>13</v>
       </c>
@@ -724,7 +733,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>0</v>
       </c>
@@ -801,7 +810,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="4" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -891,7 +900,7 @@
       <c r="AD4" s="14"/>
       <c r="AE4" s="14"/>
     </row>
-    <row r="5" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -989,7 +998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -1081,13 +1090,13 @@
         <v>59</v>
       </c>
       <c r="AD6" s="12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AE6" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -1175,17 +1184,17 @@
       <c r="AA7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC7" s="12" t="s">
+      <c r="AC7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE7" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="AD7" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE7" s="12" t="s">
-        <v>65</v>
-      </c>
     </row>
-    <row r="8" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -1273,11 +1282,17 @@
       <c r="AA8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC8" t="s">
-        <v>66</v>
+      <c r="AC8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="9" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1366,7 +1381,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1544,7 +1559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1627,7 +1642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1704,7 +1719,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1781,12 +1796,12 @@
         <v>505</v>
       </c>
       <c r="AC14" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="AD14" s="14"/>
       <c r="AE14" s="14"/>
     </row>
-    <row r="15" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1871,8 +1886,14 @@
       <c r="AE15" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="AG15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>13</v>
       </c>
@@ -1954,13 +1975,21 @@
       </c>
       <c r="AD16" s="13" t="str">
         <f>DEC2BIN(HEX2DEC(MID(AD6, 2, LEN(AD6))))</f>
-        <v>11101111</v>
+        <v>10101111</v>
       </c>
       <c r="AE16" s="12" t="s">
         <v>60</v>
       </c>
+      <c r="AG16">
+        <f t="shared" ref="AG16:AG18" ca="1" si="15">SUMPRODUCT(MID(AC16,LEN(AC16)-ROW(INDIRECT("1:"&amp;LEN(AC16)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(AC16)))-1))</f>
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <f ca="1">SUMPRODUCT(MID(AD16,LEN(AD16)-ROW(INDIRECT("1:"&amp;LEN(AD16)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(AD16)))-1))</f>
+        <v>175</v>
+      </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>14</v>
       </c>
@@ -2037,18 +2066,26 @@
         <v>902</v>
       </c>
       <c r="AC17" s="13" t="str">
-        <f>DEC2BIN(HEX2DEC(MID(AC7, 2, LEN(AC7))))</f>
-        <v>11110000</v>
+        <f t="shared" ref="AC17:AD18" si="16">DEC2BIN(HEX2DEC(MID(AC7, 2, LEN(AC7))))</f>
+        <v>10100000</v>
       </c>
       <c r="AD17" s="13" t="str">
-        <f>DEC2BIN(HEX2DEC(MID(AD7, 2, LEN(AD7))))</f>
-        <v>11111111</v>
+        <f t="shared" si="16"/>
+        <v>10101111</v>
       </c>
       <c r="AE17" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" ca="1" si="15"/>
+        <v>160</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" ref="AH17:AH18" ca="1" si="17">SUMPRODUCT(MID(AD17,LEN(AD17)-ROW(INDIRECT("1:"&amp;LEN(AD17)))+1,1)*2^(ROW(INDIRECT("1:"&amp;LEN(AD17)))-1))</f>
+        <v>175</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>15</v>
       </c>
@@ -2124,8 +2161,27 @@
         <f t="shared" ca="1" si="14"/>
         <v>8</v>
       </c>
+      <c r="AC18" s="13" t="str">
+        <f t="shared" si="16"/>
+        <v>11000000</v>
+      </c>
+      <c r="AD18" s="13" t="str">
+        <f t="shared" si="16"/>
+        <v>11111111</v>
+      </c>
+      <c r="AE18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG18">
+        <f t="shared" ca="1" si="15"/>
+        <v>192</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" ca="1" si="17"/>
+        <v>255</v>
+      </c>
     </row>
-    <row r="20" spans="2:31" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:34" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E20" s="16" t="s">
         <v>54</v>
       </c>
@@ -2137,12 +2193,12 @@
       </c>
       <c r="AE20" s="9"/>
     </row>
-    <row r="21" spans="2:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:34" ht="57.6" x14ac:dyDescent="0.3">
       <c r="U21" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
         <v>42</v>
       </c>
@@ -2165,7 +2221,7 @@
       <c r="S23" s="14"/>
       <c r="U23" s="6"/>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
         <v>43</v>
       </c>
@@ -2187,7 +2243,7 @@
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:34" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
         <v>46</v>
       </c>

</xml_diff>